<commit_message>
Tkinter project configuration implemented
</commit_message>
<xml_diff>
--- a/artifacts/model_training/results.xlsx
+++ b/artifacts/model_training/results.xlsx
@@ -497,7 +497,7 @@
         <v>28.43734500559799</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8683625768187075</v>
+        <v>4.352897191762352</v>
       </c>
     </row>
     <row r="3">
@@ -527,7 +527,7 @@
         <v>28.82105656383289</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8693849133062217</v>
+        <v>4.334840652231079</v>
       </c>
     </row>
     <row r="4">
@@ -557,67 +557,67 @@
         <v>28.85007761895036</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8694219203650375</v>
+        <v>4.333967895825444</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>XGBRegressor</t>
+          <t>CatBoostRegressor</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'learning_rate': 0.1, 'max_depth': 3, 'n_estimators': 100, 'random_state': 42, 'subsample': 0.8}</t>
+          <t>{'depth': 3, 'iterations': 1000, 'l2_leaf_reg': 1, 'learning_rate': 0.01}</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.869636058807373</v>
+        <v>0.8742270774403477</v>
       </c>
       <c r="E5" t="n">
-        <v>4.366933994293213</v>
+        <v>4.279435844213173</v>
       </c>
       <c r="F5" t="n">
-        <v>5.632278085654206</v>
+        <v>5.532213095949007</v>
       </c>
       <c r="G5" t="n">
-        <v>31.72255643414061</v>
+        <v>30.6053817389897</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8529651999473572</v>
+        <v>4.456699827494</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CatBoostRegressor</t>
+          <t>XGBRegressor</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'depth': 5, 'iterations': 1000, 'l2_leaf_reg': 3, 'learning_rate': 0.01}</t>
+          <t>{'learning_rate': 0.1, 'max_depth': 3, 'n_estimators': 100, 'random_state': 42, 'subsample': 0.8}</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.8659973357237966</v>
+        <v>0.869636058807373</v>
       </c>
       <c r="E6" t="n">
-        <v>4.367474193136229</v>
+        <v>4.366933994293213</v>
       </c>
       <c r="F6" t="n">
-        <v>5.710340963612286</v>
+        <v>5.632278085654206</v>
       </c>
       <c r="G6" t="n">
-        <v>32.60799392070849</v>
+        <v>31.72255643414061</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8609961825435398</v>
+        <v>4.624904854297638</v>
       </c>
     </row>
     <row r="7">
@@ -631,23 +631,23 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'max_depth': 10, 'min_samples_leaf': 2, 'min_samples_split': 10, 'n_estimators': 100, 'random_state': 42}</t>
+          <t>{'max_depth': None, 'min_samples_leaf': 5, 'min_samples_split': 2, 'n_estimators': 50, 'random_state': 42}</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.850382474334519</v>
+        <v>0.848044588094985</v>
       </c>
       <c r="E7" t="n">
-        <v>4.595319420439647</v>
+        <v>4.652564932331449</v>
       </c>
       <c r="F7" t="n">
-        <v>6.03387846309462</v>
+        <v>6.080837672912122</v>
       </c>
       <c r="G7" t="n">
-        <v>36.4076893073971</v>
+        <v>36.97658680430732</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8405518330742539</v>
+        <v>4.777222735225072</v>
       </c>
     </row>
     <row r="8">
@@ -677,7 +677,7 @@
         <v>37.07368383728895</v>
       </c>
       <c r="H8" t="n">
-        <v>0.8224052948218432</v>
+        <v>4.98794190290956</v>
       </c>
     </row>
     <row r="9">
@@ -707,7 +707,7 @@
         <v>40.32532946238125</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8057104066076171</v>
+        <v>5.293914599011564</v>
       </c>
     </row>
     <row r="10">
@@ -737,7 +737,7 @@
         <v>76.63957836525792</v>
       </c>
       <c r="H10" t="n">
-        <v>0.6751133216615145</v>
+        <v>6.853159430414824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented the model approval step
</commit_message>
<xml_diff>
--- a/artifacts/model_training/results.xlsx
+++ b/artifacts/model_training/results.xlsx
@@ -497,7 +497,7 @@
         <v>28.43734500559799</v>
       </c>
       <c r="H2" t="n">
-        <v>4.352897191762352</v>
+        <v>0.8683625768187075</v>
       </c>
     </row>
     <row r="3">
@@ -527,7 +527,7 @@
         <v>28.82105656383289</v>
       </c>
       <c r="H3" t="n">
-        <v>4.334840652231079</v>
+        <v>0.8693849133062217</v>
       </c>
     </row>
     <row r="4">
@@ -557,67 +557,67 @@
         <v>28.85007761895036</v>
       </c>
       <c r="H4" t="n">
-        <v>4.333967895825444</v>
+        <v>0.8694219203650375</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CatBoostRegressor</t>
+          <t>XGBRegressor</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'depth': 3, 'iterations': 1000, 'l2_leaf_reg': 1, 'learning_rate': 0.01}</t>
+          <t>{'learning_rate': 0.1, 'max_depth': 3, 'n_estimators': 100, 'random_state': 42, 'subsample': 0.8}</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.8742270774403477</v>
+        <v>0.869636058807373</v>
       </c>
       <c r="E5" t="n">
-        <v>4.279435844213173</v>
+        <v>4.366933994293213</v>
       </c>
       <c r="F5" t="n">
-        <v>5.532213095949007</v>
+        <v>5.632278085654206</v>
       </c>
       <c r="G5" t="n">
-        <v>30.6053817389897</v>
+        <v>31.72255643414061</v>
       </c>
       <c r="H5" t="n">
-        <v>4.456699827494</v>
+        <v>0.8529651999473572</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>XGBRegressor</t>
+          <t>CatBoostRegressor</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'learning_rate': 0.1, 'max_depth': 3, 'n_estimators': 100, 'random_state': 42, 'subsample': 0.8}</t>
+          <t>{'depth': 5, 'iterations': 1000, 'l2_leaf_reg': 3, 'learning_rate': 0.01}</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.869636058807373</v>
+        <v>0.8659973357237966</v>
       </c>
       <c r="E6" t="n">
-        <v>4.366933994293213</v>
+        <v>4.367474193136229</v>
       </c>
       <c r="F6" t="n">
-        <v>5.632278085654206</v>
+        <v>5.710340963612286</v>
       </c>
       <c r="G6" t="n">
-        <v>31.72255643414061</v>
+        <v>32.60799392070849</v>
       </c>
       <c r="H6" t="n">
-        <v>4.624904854297638</v>
+        <v>0.8609961825435398</v>
       </c>
     </row>
     <row r="7">
@@ -631,23 +631,23 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'max_depth': None, 'min_samples_leaf': 5, 'min_samples_split': 2, 'n_estimators': 50, 'random_state': 42}</t>
+          <t>{'max_depth': 10, 'min_samples_leaf': 2, 'min_samples_split': 10, 'n_estimators': 100, 'random_state': 42}</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.848044588094985</v>
+        <v>0.850382474334519</v>
       </c>
       <c r="E7" t="n">
-        <v>4.652564932331449</v>
+        <v>4.595319420439647</v>
       </c>
       <c r="F7" t="n">
-        <v>6.080837672912122</v>
+        <v>6.03387846309462</v>
       </c>
       <c r="G7" t="n">
-        <v>36.97658680430732</v>
+        <v>36.4076893073971</v>
       </c>
       <c r="H7" t="n">
-        <v>4.777222735225072</v>
+        <v>0.8405518330742539</v>
       </c>
     </row>
     <row r="8">
@@ -677,7 +677,7 @@
         <v>37.07368383728895</v>
       </c>
       <c r="H8" t="n">
-        <v>4.98794190290956</v>
+        <v>0.8224052948218432</v>
       </c>
     </row>
     <row r="9">
@@ -707,7 +707,7 @@
         <v>40.32532946238125</v>
       </c>
       <c r="H9" t="n">
-        <v>5.293914599011564</v>
+        <v>0.8057104066076171</v>
       </c>
     </row>
     <row r="10">
@@ -737,7 +737,7 @@
         <v>76.63957836525792</v>
       </c>
       <c r="H10" t="n">
-        <v>6.853159430414824</v>
+        <v>0.6751133216615145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>